<commit_message>
Patch for w2n and some others changes
Fixed w2n
Updated Processing: now 0 values dont recognize
updated prints.
updated tokens

Co-Authored-By: 4reeetr0 <88400860+4reeetr0@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Dictionaries/tokens.xlsx
+++ b/Dictionaries/tokens.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andri\Documents\GitHub\exchange-rates-tg-bot\Dictionaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\word-to-number-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0BD0C54-FDE1-405F-B2F4-6B6A1171F37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7E9E82-7107-4CB2-AEE5-FA41B0EF2C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
     <t>mil</t>
   </si>
   <si>
-    <t>млрд</t>
+    <t>ста</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -758,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="B138" sqref="B138:D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,7 +767,7 @@
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2033,24 +2033,24 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>134</v>
+        <v>87</v>
       </c>
       <c r="B91">
-        <v>1000000000</v>
+        <v>0</v>
       </c>
       <c r="C91">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D91">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C92">
         <v>1</v>
@@ -2061,10 +2061,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B93">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C93">
         <v>1</v>
@@ -2075,10 +2075,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B94">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C94">
         <v>1</v>
@@ -2089,10 +2089,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B95">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C95">
         <v>1</v>
@@ -2103,10 +2103,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B96">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C96">
         <v>1</v>
@@ -2117,10 +2117,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B97">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C97">
         <v>1</v>
@@ -2131,10 +2131,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B98">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C98">
         <v>1</v>
@@ -2145,10 +2145,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B99">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C99">
         <v>1</v>
@@ -2159,10 +2159,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B100">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C100">
         <v>1</v>
@@ -2173,10 +2173,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B101">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C101">
         <v>1</v>
@@ -2187,10 +2187,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B102">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C102">
         <v>1</v>
@@ -2201,10 +2201,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B103">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C103">
         <v>1</v>
@@ -2215,10 +2215,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B104">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C104">
         <v>1</v>
@@ -2229,10 +2229,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B105">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C105">
         <v>1</v>
@@ -2243,10 +2243,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B106">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C106">
         <v>1</v>
@@ -2257,10 +2257,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B107">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C107">
         <v>1</v>
@@ -2271,10 +2271,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B108">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C108">
         <v>1</v>
@@ -2285,10 +2285,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B109">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -2299,10 +2299,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B110">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C110">
         <v>1</v>
@@ -2313,13 +2313,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B111">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C111">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D111">
         <v>0</v>
@@ -2327,10 +2327,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B112">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C112">
         <v>2</v>
@@ -2341,10 +2341,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B113">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C113">
         <v>2</v>
@@ -2355,10 +2355,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B114">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C114">
         <v>2</v>
@@ -2369,10 +2369,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B115">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C115">
         <v>2</v>
@@ -2383,10 +2383,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B116">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C116">
         <v>2</v>
@@ -2397,10 +2397,10 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B117">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C117">
         <v>2</v>
@@ -2411,10 +2411,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B118">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C118">
         <v>2</v>
@@ -2425,27 +2425,27 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B119">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C119">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D119">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B120">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C120">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D120">
         <v>1</v>
@@ -2453,7 +2453,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B121">
         <v>1000</v>
@@ -2467,7 +2467,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B122">
         <v>1000</v>
@@ -2481,13 +2481,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B123">
-        <v>1000</v>
+        <v>1000000</v>
       </c>
       <c r="C123">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D123">
         <v>1</v>
@@ -2495,7 +2495,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B124">
         <v>1000000</v>
@@ -2509,13 +2509,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B125">
-        <v>1000000</v>
+        <v>1000000000</v>
       </c>
       <c r="C125">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D125">
         <v>1</v>
@@ -2523,7 +2523,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B126">
         <v>1000000000</v>
@@ -2537,13 +2537,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B127">
-        <v>1000000000</v>
+        <v>12</v>
       </c>
       <c r="C127">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D127">
         <v>1</v>
@@ -2551,13 +2551,13 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B128">
-        <v>12</v>
+        <v>1000</v>
       </c>
       <c r="C128">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D128">
         <v>1</v>
@@ -2565,13 +2565,13 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B129">
-        <v>1000</v>
+        <v>1000000</v>
       </c>
       <c r="C129">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D129">
         <v>1</v>
@@ -2579,13 +2579,13 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B130">
-        <v>1000000</v>
+        <v>1000000000</v>
       </c>
       <c r="C130">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D130">
         <v>1</v>
@@ -2593,13 +2593,13 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B131">
-        <v>1000000000</v>
+        <v>1000000000000</v>
       </c>
       <c r="C131">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D131">
         <v>1</v>
@@ -2607,7 +2607,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B132">
         <v>1000000000000</v>
@@ -2621,7 +2621,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B133">
         <v>1000000000000</v>
@@ -2635,13 +2635,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B134">
-        <v>1000000000000</v>
+        <v>1000</v>
       </c>
       <c r="C134">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D134">
         <v>1</v>
@@ -2649,7 +2649,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B135">
         <v>1000</v>
@@ -2663,13 +2663,13 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B136">
-        <v>1000</v>
+        <v>1000000</v>
       </c>
       <c r="C136">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D136">
         <v>1</v>
@@ -2677,13 +2677,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B137">
-        <v>1000000000</v>
+        <v>1000000</v>
       </c>
       <c r="C137">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D137">
         <v>1</v>
@@ -2691,16 +2691,16 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B138">
-        <v>1000000000</v>
+        <v>100</v>
       </c>
       <c r="C138">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D138">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>